<commit_message>
performance trends - lines - v1
</commit_message>
<xml_diff>
--- a/Base_Data/Excel+ALL+ENG.xlsx
+++ b/Base_Data/Excel+ALL+ENG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex.y/Documents/Github_Repo/G10_CTB_Global-Finals_Data-Analysis/Base_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C1F95A-7FEB-EE42-87B4-A57458AE6920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154168C9-F4BC-AF40-AFFB-0CE0A12777B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="31720" windowHeight="22500" xr2:uid="{98D09DEC-93DB-E744-8CBC-B24D25E4341D}"/>
   </bookViews>
@@ -178,15 +178,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Social Interaction Mean Score	</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Emotion Regulation Mean Score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall Daily Performance Mean Score	</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -195,6 +187,14 @@
   </si>
   <si>
     <t>Repetitive Behaviors and Interests Mean Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social Interaction Mean Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall Daily Performance Mean Score</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -283,9 +283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -296,6 +293,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0A3F08-FF35-D14B-A48B-730CB434908B}">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="AK32" sqref="AK32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -703,16 +703,17 @@
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="12" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="32.1640625" style="7" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="58.6640625" style="6" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="8.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="23" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="19.83203125" style="7" customWidth="1" collapsed="1"/>
-    <col min="25" max="30" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="21.33203125" style="7" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="34.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="25" max="29" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="20.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="39.33203125" style="6" customWidth="1" collapsed="1"/>
     <col min="32" max="35" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="28.1640625" style="7" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="24" style="7" customWidth="1"/>
-    <col min="38" max="38" width="31.1640625" style="7" customWidth="1"/>
+    <col min="36" max="36" width="42.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="38.6640625" style="6" customWidth="1"/>
+    <col min="38" max="38" width="68.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="36" customHeight="1">
@@ -752,7 +753,7 @@
       <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="8" t="s">
         <v>34</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -785,8 +786,8 @@
       <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>35</v>
+      <c r="X1" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>19</v>
@@ -806,8 +807,8 @@
       <c r="AD1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="4" t="s">
-        <v>36</v>
+      <c r="AE1" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>25</v>
@@ -821,14 +822,14 @@
       <c r="AI1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL1" s="4" t="s">
-        <v>38</v>
+      <c r="AL1" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -838,7 +839,7 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="3">
@@ -866,7 +867,7 @@
       <c r="L2" s="3">
         <v>8</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <f t="shared" ref="M2:M51" si="0">AVERAGE(D2:L2)</f>
         <v>7.125</v>
       </c>
@@ -896,7 +897,7 @@
       <c r="W2" s="3">
         <v>7</v>
       </c>
-      <c r="X2" s="5">
+      <c r="X2" s="4">
         <f t="shared" ref="X2:X51" si="1">AVERAGE(N2:W2)</f>
         <v>6.75</v>
       </c>
@@ -916,7 +917,7 @@
       <c r="AD2" s="3">
         <v>9</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AE2" s="4">
         <f t="shared" ref="AE2:AE51" si="2">AVERAGE(Y2:AD2)</f>
         <v>8.1999999999999993</v>
       </c>
@@ -932,15 +933,15 @@
       <c r="AI2" s="3">
         <v>7</v>
       </c>
-      <c r="AJ2" s="5">
+      <c r="AJ2" s="4">
         <f t="shared" ref="AJ2:AJ51" si="3">AVERAGE(AF2:AI2)</f>
         <v>4.75</v>
       </c>
-      <c r="AK2" s="5">
+      <c r="AK2" s="4">
         <f t="shared" ref="AK2:AK51" si="4">AVERAGE(D2:L2,N2:W2,Y2:AD2,AF2:AI2)</f>
         <v>6.84</v>
       </c>
-      <c r="AL2" s="6"/>
+      <c r="AL2" s="5"/>
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="3">
@@ -949,7 +950,7 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="3">
@@ -977,7 +978,7 @@
       <c r="L3" s="3">
         <v>6</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <f t="shared" si="0"/>
         <v>7.125</v>
       </c>
@@ -1007,7 +1008,7 @@
       <c r="W3" s="3">
         <v>8</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3" s="4">
         <f t="shared" si="1"/>
         <v>6.875</v>
       </c>
@@ -1021,7 +1022,7 @@
       </c>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-      <c r="AE3" s="5">
+      <c r="AE3" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -1037,15 +1038,15 @@
       <c r="AI3" s="3">
         <v>5</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AJ3" s="4">
         <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
-      <c r="AK3" s="5">
+      <c r="AK3" s="4">
         <f t="shared" si="4"/>
         <v>6.6818181818181817</v>
       </c>
-      <c r="AL3" s="6"/>
+      <c r="AL3" s="5"/>
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="3">
@@ -1054,7 +1055,7 @@
       <c r="B4" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="3"/>
@@ -1072,7 +1073,7 @@
       <c r="L4" s="3">
         <v>8</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1098,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="W4" s="3"/>
-      <c r="X4" s="5">
+      <c r="X4" s="4">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
@@ -1112,7 +1113,7 @@
       <c r="AD4" s="3">
         <v>10</v>
       </c>
-      <c r="AE4" s="5">
+      <c r="AE4" s="4">
         <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
@@ -1126,15 +1127,15 @@
       <c r="AI4" s="3">
         <v>8</v>
       </c>
-      <c r="AJ4" s="5">
+      <c r="AJ4" s="4">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="AK4" s="5">
+      <c r="AK4" s="4">
         <f t="shared" si="4"/>
         <v>7.7857142857142856</v>
       </c>
-      <c r="AL4" s="6"/>
+      <c r="AL4" s="5"/>
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="3">
@@ -1143,7 +1144,7 @@
       <c r="B5" s="3">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="3"/>
@@ -1159,7 +1160,7 @@
       <c r="L5" s="3">
         <v>9</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>9</v>
       </c>
       <c r="W5" s="3"/>
-      <c r="X5" s="5">
+      <c r="X5" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -1193,7 +1194,7 @@
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="5">
+      <c r="AE5" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -1205,15 +1206,15 @@
         <v>7</v>
       </c>
       <c r="AI5" s="3"/>
-      <c r="AJ5" s="5">
+      <c r="AJ5" s="4">
         <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
-      <c r="AK5" s="5">
+      <c r="AK5" s="4">
         <f t="shared" si="4"/>
         <v>7.8888888888888893</v>
       </c>
-      <c r="AL5" s="6">
+      <c r="AL5" s="5">
         <f>AK5-AK2</f>
         <v>1.0488888888888894</v>
       </c>
@@ -1225,7 +1226,7 @@
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="3">
@@ -1253,7 +1254,7 @@
       <c r="L6" s="3">
         <v>8</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <f t="shared" si="0"/>
         <v>7.875</v>
       </c>
@@ -1287,7 +1288,7 @@
       <c r="W6" s="3">
         <v>4</v>
       </c>
-      <c r="X6" s="5">
+      <c r="X6" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1299,7 +1300,7 @@
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="5">
+      <c r="AE6" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -1315,15 +1316,15 @@
       <c r="AI6" s="3">
         <v>6</v>
       </c>
-      <c r="AJ6" s="5">
+      <c r="AJ6" s="4">
         <f t="shared" si="3"/>
         <v>4.25</v>
       </c>
-      <c r="AK6" s="5">
+      <c r="AK6" s="4">
         <f t="shared" si="4"/>
         <v>5.7391304347826084</v>
       </c>
-      <c r="AL6" s="6"/>
+      <c r="AL6" s="5"/>
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="3">
@@ -1332,7 +1333,7 @@
       <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="3">
@@ -1360,7 +1361,7 @@
       <c r="L7" s="3">
         <v>8</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <f t="shared" si="0"/>
         <v>6.375</v>
       </c>
@@ -1394,7 +1395,7 @@
       <c r="W7" s="3">
         <v>3</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7" s="4">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
@@ -1410,7 +1411,7 @@
       <c r="AD7" s="3">
         <v>8</v>
       </c>
-      <c r="AE7" s="5">
+      <c r="AE7" s="4">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -1426,15 +1427,15 @@
       <c r="AI7" s="3">
         <v>4</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7" s="4">
         <f t="shared" si="3"/>
         <v>4.25</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AK7" s="4">
         <f t="shared" si="4"/>
         <v>5.36</v>
       </c>
-      <c r="AL7" s="6"/>
+      <c r="AL7" s="5"/>
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="3">
@@ -1443,7 +1444,7 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="3">
@@ -1469,7 +1470,7 @@
       <c r="L8" s="3">
         <v>6</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <f t="shared" si="0"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1497,7 +1498,7 @@
       <c r="W8" s="3">
         <v>5</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="4">
         <f t="shared" si="1"/>
         <v>5.5714285714285712</v>
       </c>
@@ -1513,7 +1514,7 @@
       <c r="AD8" s="3">
         <v>8</v>
       </c>
-      <c r="AE8" s="5">
+      <c r="AE8" s="4">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -1529,15 +1530,15 @@
       <c r="AI8" s="3">
         <v>6</v>
       </c>
-      <c r="AJ8" s="5">
+      <c r="AJ8" s="4">
         <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
-      <c r="AK8" s="5">
+      <c r="AK8" s="4">
         <f t="shared" si="4"/>
         <v>5.666666666666667</v>
       </c>
-      <c r="AL8" s="6"/>
+      <c r="AL8" s="5"/>
     </row>
     <row r="9" spans="1:38">
       <c r="A9" s="3">
@@ -1546,7 +1547,7 @@
       <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="3">
@@ -1574,7 +1575,7 @@
       <c r="L9" s="3">
         <v>7</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <f t="shared" si="0"/>
         <v>6.75</v>
       </c>
@@ -1606,7 +1607,7 @@
       <c r="W9" s="3">
         <v>4</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="4">
         <f t="shared" si="1"/>
         <v>4.8888888888888893</v>
       </c>
@@ -1626,7 +1627,7 @@
       <c r="AD9" s="3">
         <v>9</v>
       </c>
-      <c r="AE9" s="5">
+      <c r="AE9" s="4">
         <f t="shared" si="2"/>
         <v>5.4</v>
       </c>
@@ -1642,15 +1643,15 @@
       <c r="AI9" s="3">
         <v>3</v>
       </c>
-      <c r="AJ9" s="5">
+      <c r="AJ9" s="4">
         <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
-      <c r="AK9" s="5">
+      <c r="AK9" s="4">
         <f t="shared" si="4"/>
         <v>5.384615384615385</v>
       </c>
-      <c r="AL9" s="6"/>
+      <c r="AL9" s="5"/>
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="3">
@@ -1659,7 +1660,7 @@
       <c r="B10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="3">
@@ -1679,7 +1680,7 @@
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1713,7 +1714,7 @@
       <c r="W10" s="3">
         <v>3</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="4">
         <f t="shared" si="1"/>
         <v>6.3</v>
       </c>
@@ -1735,7 +1736,7 @@
       <c r="AD10" s="3">
         <v>8</v>
       </c>
-      <c r="AE10" s="5">
+      <c r="AE10" s="4">
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
@@ -1751,15 +1752,15 @@
       <c r="AI10" s="3">
         <v>4</v>
       </c>
-      <c r="AJ10" s="5">
+      <c r="AJ10" s="4">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="AK10" s="5">
+      <c r="AK10" s="4">
         <f t="shared" si="4"/>
         <v>6.166666666666667</v>
       </c>
-      <c r="AL10" s="6">
+      <c r="AL10" s="5">
         <f>AK10-AK6</f>
         <v>0.42753623188405854</v>
       </c>
@@ -1771,7 +1772,7 @@
       <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3">
@@ -1799,7 +1800,7 @@
       <c r="L11" s="3">
         <v>7</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>7</v>
       </c>
       <c r="W11" s="3"/>
-      <c r="X11" s="5">
+      <c r="X11" s="4">
         <f t="shared" si="1"/>
         <v>6.7142857142857144</v>
       </c>
@@ -1847,7 +1848,7 @@
       <c r="AD11" s="3">
         <v>8</v>
       </c>
-      <c r="AE11" s="5">
+      <c r="AE11" s="4">
         <f t="shared" si="2"/>
         <v>7.2</v>
       </c>
@@ -1863,15 +1864,15 @@
       <c r="AI11" s="3">
         <v>5</v>
       </c>
-      <c r="AJ11" s="5">
+      <c r="AJ11" s="4">
         <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="AK11" s="5">
+      <c r="AK11" s="4">
         <f t="shared" si="4"/>
         <v>6.208333333333333</v>
       </c>
-      <c r="AL11" s="6"/>
+      <c r="AL11" s="5"/>
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="3">
@@ -1880,7 +1881,7 @@
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="3">
@@ -1906,7 +1907,7 @@
       <c r="L12" s="3">
         <v>8</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <f t="shared" si="0"/>
         <v>6.8571428571428568</v>
       </c>
@@ -1940,7 +1941,7 @@
       <c r="W12" s="3">
         <v>7</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="4">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
@@ -1956,7 +1957,7 @@
       </c>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="5">
+      <c r="AE12" s="4">
         <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
@@ -1972,15 +1973,15 @@
       <c r="AI12" s="3">
         <v>8</v>
       </c>
-      <c r="AJ12" s="5">
+      <c r="AJ12" s="4">
         <f t="shared" si="3"/>
         <v>6.25</v>
       </c>
-      <c r="AK12" s="5">
+      <c r="AK12" s="4">
         <f t="shared" si="4"/>
         <v>7.25</v>
       </c>
-      <c r="AL12" s="6"/>
+      <c r="AL12" s="5"/>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="3">
@@ -1989,7 +1990,7 @@
       <c r="B13" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="3">
@@ -2015,7 +2016,7 @@
       <c r="L13" s="3">
         <v>9</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <f t="shared" si="0"/>
         <v>7.4285714285714288</v>
       </c>
@@ -2049,7 +2050,7 @@
       <c r="W13" s="3">
         <v>7</v>
       </c>
-      <c r="X13" s="5">
+      <c r="X13" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>10</v>
       </c>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="5">
+      <c r="AE13" s="4">
         <f t="shared" si="2"/>
         <v>8.75</v>
       </c>
@@ -2083,15 +2084,15 @@
       <c r="AI13" s="3">
         <v>9</v>
       </c>
-      <c r="AJ13" s="5">
+      <c r="AJ13" s="4">
         <f t="shared" si="3"/>
         <v>7.25</v>
       </c>
-      <c r="AK13" s="5">
+      <c r="AK13" s="4">
         <f t="shared" si="4"/>
         <v>7.84</v>
       </c>
-      <c r="AL13" s="6"/>
+      <c r="AL13" s="5"/>
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="3">
@@ -2100,7 +2101,7 @@
       <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="3">
@@ -2126,7 +2127,7 @@
       <c r="L14" s="3">
         <v>9</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="4">
         <f t="shared" si="0"/>
         <v>7.7142857142857144</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>8</v>
       </c>
       <c r="W14" s="3"/>
-      <c r="X14" s="5">
+      <c r="X14" s="4">
         <f t="shared" si="1"/>
         <v>7.7777777777777777</v>
       </c>
@@ -2174,7 +2175,7 @@
       <c r="AD14" s="3">
         <v>7</v>
       </c>
-      <c r="AE14" s="5">
+      <c r="AE14" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -2190,15 +2191,15 @@
       <c r="AI14" s="3">
         <v>9</v>
       </c>
-      <c r="AJ14" s="5">
+      <c r="AJ14" s="4">
         <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
-      <c r="AK14" s="5">
+      <c r="AK14" s="4">
         <f t="shared" si="4"/>
         <v>7.7391304347826084</v>
       </c>
-      <c r="AL14" s="6"/>
+      <c r="AL14" s="5"/>
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="3">
@@ -2207,7 +2208,7 @@
       <c r="B15" s="3">
         <v>5</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="3"/>
@@ -2227,7 +2228,7 @@
         <v>9</v>
       </c>
       <c r="L15" s="3"/>
-      <c r="M15" s="5">
+      <c r="M15" s="4">
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
@@ -2257,7 +2258,7 @@
       <c r="W15" s="3">
         <v>8</v>
       </c>
-      <c r="X15" s="5">
+      <c r="X15" s="4">
         <f t="shared" si="1"/>
         <v>7.875</v>
       </c>
@@ -2273,7 +2274,7 @@
       </c>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
-      <c r="AE15" s="5">
+      <c r="AE15" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -2289,15 +2290,15 @@
       <c r="AI15" s="3">
         <v>7</v>
       </c>
-      <c r="AJ15" s="5">
+      <c r="AJ15" s="4">
         <f t="shared" si="3"/>
         <v>7.5</v>
       </c>
-      <c r="AK15" s="5">
+      <c r="AK15" s="4">
         <f t="shared" si="4"/>
         <v>7.7894736842105265</v>
       </c>
-      <c r="AL15" s="6">
+      <c r="AL15" s="5">
         <f>AK15-AK11</f>
         <v>1.5811403508771935</v>
       </c>
@@ -2309,7 +2310,7 @@
       <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="3">
@@ -2337,7 +2338,7 @@
       <c r="L16" s="3">
         <v>1</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="4">
         <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
@@ -2371,7 +2372,7 @@
       <c r="W16" s="3">
         <v>2</v>
       </c>
-      <c r="X16" s="5">
+      <c r="X16" s="4">
         <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
@@ -2393,7 +2394,7 @@
       <c r="AD16" s="3">
         <v>9</v>
       </c>
-      <c r="AE16" s="5">
+      <c r="AE16" s="4">
         <f t="shared" si="2"/>
         <v>5.166666666666667</v>
       </c>
@@ -2409,15 +2410,15 @@
       <c r="AI16" s="3">
         <v>0</v>
       </c>
-      <c r="AJ16" s="5">
+      <c r="AJ16" s="4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AK16" s="5">
+      <c r="AK16" s="4">
         <f t="shared" si="4"/>
         <v>3.0714285714285716</v>
       </c>
-      <c r="AL16" s="6"/>
+      <c r="AL16" s="5"/>
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="3">
@@ -2426,7 +2427,7 @@
       <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="3">
@@ -2454,7 +2455,7 @@
       <c r="L17" s="3">
         <v>4</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="4">
         <f t="shared" si="0"/>
         <v>4.625</v>
       </c>
@@ -2488,7 +2489,7 @@
       <c r="W17" s="3">
         <v>6</v>
       </c>
-      <c r="X17" s="5">
+      <c r="X17" s="4">
         <f t="shared" si="1"/>
         <v>3.8</v>
       </c>
@@ -2510,7 +2511,7 @@
       <c r="AD17" s="3">
         <v>10</v>
       </c>
-      <c r="AE17" s="5">
+      <c r="AE17" s="4">
         <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
@@ -2526,15 +2527,15 @@
       <c r="AI17" s="3">
         <v>1</v>
       </c>
-      <c r="AJ17" s="5">
+      <c r="AJ17" s="4">
         <f t="shared" si="3"/>
         <v>2.25</v>
       </c>
-      <c r="AK17" s="5">
+      <c r="AK17" s="4">
         <f t="shared" si="4"/>
         <v>4.3928571428571432</v>
       </c>
-      <c r="AL17" s="6"/>
+      <c r="AL17" s="5"/>
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="3">
@@ -2543,7 +2544,7 @@
       <c r="B18" s="3">
         <v>3</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="3">
@@ -2571,7 +2572,7 @@
       <c r="L18" s="3">
         <v>6</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="4">
         <f t="shared" si="0"/>
         <v>6.625</v>
       </c>
@@ -2605,7 +2606,7 @@
       <c r="W18" s="3">
         <v>7</v>
       </c>
-      <c r="X18" s="5">
+      <c r="X18" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -2627,7 +2628,7 @@
       <c r="AD18" s="3">
         <v>10</v>
       </c>
-      <c r="AE18" s="5">
+      <c r="AE18" s="4">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -2643,15 +2644,15 @@
       <c r="AI18" s="3">
         <v>2</v>
       </c>
-      <c r="AJ18" s="5">
+      <c r="AJ18" s="4">
         <f t="shared" si="3"/>
         <v>2.75</v>
       </c>
-      <c r="AK18" s="5">
+      <c r="AK18" s="4">
         <f t="shared" si="4"/>
         <v>5.5714285714285712</v>
       </c>
-      <c r="AL18" s="6"/>
+      <c r="AL18" s="5"/>
     </row>
     <row r="19" spans="1:38">
       <c r="A19" s="3">
@@ -2660,7 +2661,7 @@
       <c r="B19" s="3">
         <v>4</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="3">
@@ -2688,7 +2689,7 @@
       <c r="L19" s="3">
         <v>7</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2722,7 +2723,7 @@
       <c r="W19" s="3">
         <v>8</v>
       </c>
-      <c r="X19" s="5">
+      <c r="X19" s="4">
         <f t="shared" si="1"/>
         <v>5.9</v>
       </c>
@@ -2744,7 +2745,7 @@
       <c r="AD19" s="3">
         <v>10</v>
       </c>
-      <c r="AE19" s="5">
+      <c r="AE19" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -2760,15 +2761,15 @@
       <c r="AI19" s="3">
         <v>4</v>
       </c>
-      <c r="AJ19" s="5">
+      <c r="AJ19" s="4">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="AK19" s="5">
+      <c r="AK19" s="4">
         <f t="shared" si="4"/>
         <v>6.3928571428571432</v>
       </c>
-      <c r="AL19" s="6"/>
+      <c r="AL19" s="5"/>
     </row>
     <row r="20" spans="1:38">
       <c r="A20" s="3">
@@ -2777,7 +2778,7 @@
       <c r="B20" s="3">
         <v>5</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="3">
@@ -2807,7 +2808,7 @@
       <c r="L20" s="3">
         <v>6</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="4">
         <f t="shared" si="0"/>
         <v>7.2222222222222223</v>
       </c>
@@ -2841,7 +2842,7 @@
       <c r="W20" s="3">
         <v>6</v>
       </c>
-      <c r="X20" s="5">
+      <c r="X20" s="4">
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
@@ -2863,7 +2864,7 @@
       <c r="AD20" s="3">
         <v>10</v>
       </c>
-      <c r="AE20" s="5">
+      <c r="AE20" s="4">
         <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
@@ -2879,15 +2880,15 @@
       <c r="AI20" s="3">
         <v>5</v>
       </c>
-      <c r="AJ20" s="5">
+      <c r="AJ20" s="4">
         <f t="shared" si="3"/>
         <v>5.25</v>
       </c>
-      <c r="AK20" s="5">
+      <c r="AK20" s="4">
         <f t="shared" si="4"/>
         <v>6.8620689655172411</v>
       </c>
-      <c r="AL20" s="6">
+      <c r="AL20" s="5">
         <f>AK20-AK16</f>
         <v>3.7906403940886695</v>
       </c>
@@ -2899,7 +2900,7 @@
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="3">
@@ -2929,7 +2930,7 @@
       <c r="L21" s="3">
         <v>7</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="4">
         <f t="shared" si="0"/>
         <v>6.1111111111111107</v>
       </c>
@@ -2963,7 +2964,7 @@
       <c r="W21" s="3">
         <v>3</v>
       </c>
-      <c r="X21" s="5">
+      <c r="X21" s="4">
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
@@ -2983,7 +2984,7 @@
       <c r="AD21" s="3">
         <v>8</v>
       </c>
-      <c r="AE21" s="5">
+      <c r="AE21" s="4">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -2999,15 +3000,15 @@
       <c r="AI21" s="3">
         <v>7</v>
       </c>
-      <c r="AJ21" s="5">
+      <c r="AJ21" s="4">
         <f t="shared" si="3"/>
         <v>6.75</v>
       </c>
-      <c r="AK21" s="5">
+      <c r="AK21" s="4">
         <f t="shared" si="4"/>
         <v>6.2142857142857144</v>
       </c>
-      <c r="AL21" s="6"/>
+      <c r="AL21" s="5"/>
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="3">
@@ -3016,7 +3017,7 @@
       <c r="B22" s="3">
         <v>2</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="3">
@@ -3044,7 +3045,7 @@
       <c r="L22" s="3">
         <v>7</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -3078,7 +3079,7 @@
       <c r="W22" s="3">
         <v>7</v>
       </c>
-      <c r="X22" s="5">
+      <c r="X22" s="4">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
@@ -3098,7 +3099,7 @@
       <c r="AD22" s="3">
         <v>8</v>
       </c>
-      <c r="AE22" s="5">
+      <c r="AE22" s="4">
         <f t="shared" si="2"/>
         <v>7.4</v>
       </c>
@@ -3114,15 +3115,15 @@
       <c r="AI22" s="3">
         <v>6</v>
       </c>
-      <c r="AJ22" s="5">
+      <c r="AJ22" s="4">
         <f t="shared" si="3"/>
         <v>7.25</v>
       </c>
-      <c r="AK22" s="5">
+      <c r="AK22" s="4">
         <f t="shared" si="4"/>
         <v>7.2962962962962967</v>
       </c>
-      <c r="AL22" s="6"/>
+      <c r="AL22" s="5"/>
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="3">
@@ -3131,7 +3132,7 @@
       <c r="B23" s="3">
         <v>3</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="3">
@@ -3159,7 +3160,7 @@
       <c r="L23" s="3">
         <v>9</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="4">
         <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
@@ -3193,7 +3194,7 @@
       <c r="W23" s="3">
         <v>6</v>
       </c>
-      <c r="X23" s="5">
+      <c r="X23" s="4">
         <f t="shared" si="1"/>
         <v>7.8</v>
       </c>
@@ -3215,7 +3216,7 @@
       <c r="AD23" s="3">
         <v>8</v>
       </c>
-      <c r="AE23" s="5">
+      <c r="AE23" s="4">
         <f t="shared" si="2"/>
         <v>7.666666666666667</v>
       </c>
@@ -3231,15 +3232,15 @@
       <c r="AI23" s="3">
         <v>8</v>
       </c>
-      <c r="AJ23" s="5">
+      <c r="AJ23" s="4">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="AK23" s="5">
+      <c r="AK23" s="4">
         <f t="shared" si="4"/>
         <v>7.8928571428571432</v>
       </c>
-      <c r="AL23" s="6"/>
+      <c r="AL23" s="5"/>
     </row>
     <row r="24" spans="1:38">
       <c r="A24" s="3">
@@ -3248,7 +3249,7 @@
       <c r="B24" s="3">
         <v>4</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="3">
@@ -3278,7 +3279,7 @@
       <c r="L24" s="3">
         <v>10</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="4">
         <f t="shared" si="0"/>
         <v>7.666666666666667</v>
       </c>
@@ -3312,7 +3313,7 @@
       <c r="W24" s="3">
         <v>5</v>
       </c>
-      <c r="X24" s="5">
+      <c r="X24" s="4">
         <f t="shared" si="1"/>
         <v>7.8</v>
       </c>
@@ -3334,7 +3335,7 @@
       <c r="AD24" s="3">
         <v>8</v>
       </c>
-      <c r="AE24" s="5">
+      <c r="AE24" s="4">
         <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
@@ -3350,15 +3351,15 @@
       <c r="AI24" s="3">
         <v>7</v>
       </c>
-      <c r="AJ24" s="5">
+      <c r="AJ24" s="4">
         <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
-      <c r="AK24" s="5">
+      <c r="AK24" s="4">
         <f t="shared" si="4"/>
         <v>8.0344827586206904</v>
       </c>
-      <c r="AL24" s="6"/>
+      <c r="AL24" s="5"/>
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="3">
@@ -3367,7 +3368,7 @@
       <c r="B25" s="3">
         <v>5</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="3">
@@ -3397,7 +3398,7 @@
       <c r="L25" s="3">
         <v>10</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="4">
         <f t="shared" si="0"/>
         <v>8.4444444444444446</v>
       </c>
@@ -3431,7 +3432,7 @@
       <c r="W25" s="3">
         <v>7</v>
       </c>
-      <c r="X25" s="5">
+      <c r="X25" s="4">
         <f t="shared" si="1"/>
         <v>8.9</v>
       </c>
@@ -3453,7 +3454,7 @@
       <c r="AD25" s="3">
         <v>8</v>
       </c>
-      <c r="AE25" s="5">
+      <c r="AE25" s="4">
         <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
@@ -3469,15 +3470,15 @@
       <c r="AI25" s="3">
         <v>7</v>
       </c>
-      <c r="AJ25" s="5">
+      <c r="AJ25" s="4">
         <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
-      <c r="AK25" s="5">
+      <c r="AK25" s="4">
         <f t="shared" si="4"/>
         <v>8.6551724137931032</v>
       </c>
-      <c r="AL25" s="6">
+      <c r="AL25" s="5">
         <f>AK25-AK21</f>
         <v>2.4408866995073888</v>
       </c>
@@ -3489,7 +3490,7 @@
       <c r="B26" s="3">
         <v>1</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="3">
@@ -3519,7 +3520,7 @@
       <c r="L26" s="3">
         <v>2</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="4">
         <f t="shared" si="0"/>
         <v>6.5555555555555554</v>
       </c>
@@ -3553,7 +3554,7 @@
       <c r="W26" s="3">
         <v>7</v>
       </c>
-      <c r="X26" s="5">
+      <c r="X26" s="4">
         <f t="shared" si="1"/>
         <v>2.9</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>7</v>
       </c>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="5">
+      <c r="AE26" s="4">
         <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
@@ -3589,15 +3590,15 @@
       <c r="AI26" s="3">
         <v>3</v>
       </c>
-      <c r="AJ26" s="5">
+      <c r="AJ26" s="4">
         <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
-      <c r="AK26" s="5">
+      <c r="AK26" s="4">
         <f t="shared" si="4"/>
         <v>4.5714285714285712</v>
       </c>
-      <c r="AL26" s="6"/>
+      <c r="AL26" s="5"/>
     </row>
     <row r="27" spans="1:38">
       <c r="A27" s="3">
@@ -3606,7 +3607,7 @@
       <c r="B27" s="3">
         <v>2</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="3">
@@ -3634,7 +3635,7 @@
       <c r="L27" s="3">
         <v>1</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27" s="4">
         <f t="shared" si="0"/>
         <v>3.875</v>
       </c>
@@ -3668,7 +3669,7 @@
       <c r="W27" s="3">
         <v>9</v>
       </c>
-      <c r="X27" s="5">
+      <c r="X27" s="4">
         <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>7</v>
       </c>
       <c r="AD27" s="3"/>
-      <c r="AE27" s="5">
+      <c r="AE27" s="4">
         <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
@@ -3704,15 +3705,15 @@
       <c r="AI27" s="3">
         <v>1</v>
       </c>
-      <c r="AJ27" s="5">
+      <c r="AJ27" s="4">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="AK27" s="5">
+      <c r="AK27" s="4">
         <f t="shared" si="4"/>
         <v>3.5185185185185186</v>
       </c>
-      <c r="AL27" s="6"/>
+      <c r="AL27" s="5"/>
     </row>
     <row r="28" spans="1:38">
       <c r="A28" s="3">
@@ -3721,7 +3722,7 @@
       <c r="B28" s="3">
         <v>3</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="3">
@@ -3747,7 +3748,7 @@
       <c r="L28" s="3">
         <v>2</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="4">
         <f t="shared" si="0"/>
         <v>4.1428571428571432</v>
       </c>
@@ -3781,7 +3782,7 @@
       <c r="W28" s="3">
         <v>9</v>
       </c>
-      <c r="X28" s="5">
+      <c r="X28" s="4">
         <f t="shared" si="1"/>
         <v>3.9</v>
       </c>
@@ -3801,7 +3802,7 @@
         <v>7</v>
       </c>
       <c r="AD28" s="3"/>
-      <c r="AE28" s="5">
+      <c r="AE28" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -3817,15 +3818,15 @@
       <c r="AI28" s="3">
         <v>1</v>
       </c>
-      <c r="AJ28" s="5">
+      <c r="AJ28" s="4">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="AK28" s="5">
+      <c r="AK28" s="4">
         <f t="shared" si="4"/>
         <v>3.6923076923076925</v>
       </c>
-      <c r="AL28" s="6"/>
+      <c r="AL28" s="5"/>
     </row>
     <row r="29" spans="1:38">
       <c r="A29" s="3">
@@ -3834,7 +3835,7 @@
       <c r="B29" s="3">
         <v>4</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="3">
@@ -3862,7 +3863,7 @@
       <c r="L29" s="3">
         <v>3</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3896,7 +3897,7 @@
       <c r="W29" s="3">
         <v>10</v>
       </c>
-      <c r="X29" s="5">
+      <c r="X29" s="4">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
@@ -3916,7 +3917,7 @@
         <v>8</v>
       </c>
       <c r="AD29" s="3"/>
-      <c r="AE29" s="5">
+      <c r="AE29" s="4">
         <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
@@ -3932,15 +3933,15 @@
       <c r="AI29" s="3">
         <v>1</v>
       </c>
-      <c r="AJ29" s="5">
+      <c r="AJ29" s="4">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="AK29" s="5">
+      <c r="AK29" s="4">
         <f t="shared" si="4"/>
         <v>3.8888888888888888</v>
       </c>
-      <c r="AL29" s="6"/>
+      <c r="AL29" s="5"/>
     </row>
     <row r="30" spans="1:38">
       <c r="A30" s="3">
@@ -3949,7 +3950,7 @@
       <c r="B30" s="3">
         <v>5</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="3"/>
@@ -3969,7 +3970,7 @@
       <c r="L30" s="3">
         <v>6</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30" s="4">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
@@ -4001,7 +4002,7 @@
       <c r="W30" s="3">
         <v>10</v>
       </c>
-      <c r="X30" s="5">
+      <c r="X30" s="4">
         <f t="shared" si="1"/>
         <v>6.1111111111111107</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>8</v>
       </c>
       <c r="AD30" s="3"/>
-      <c r="AE30" s="5">
+      <c r="AE30" s="4">
         <f t="shared" si="2"/>
         <v>6.4</v>
       </c>
@@ -4037,15 +4038,15 @@
       <c r="AI30" s="3">
         <v>3</v>
       </c>
-      <c r="AJ30" s="5">
+      <c r="AJ30" s="4">
         <f t="shared" si="3"/>
         <v>3.25</v>
       </c>
-      <c r="AK30" s="5">
+      <c r="AK30" s="4">
         <f t="shared" si="4"/>
         <v>5.6818181818181817</v>
       </c>
-      <c r="AL30" s="6">
+      <c r="AL30" s="5">
         <f>AK30-AK26</f>
         <v>1.1103896103896105</v>
       </c>
@@ -4057,7 +4058,7 @@
       <c r="B31" s="3">
         <v>1</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="3">
@@ -4085,7 +4086,7 @@
       <c r="L31" s="3">
         <v>7</v>
       </c>
-      <c r="M31" s="5">
+      <c r="M31" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -4117,7 +4118,7 @@
       <c r="W31" s="3">
         <v>6</v>
       </c>
-      <c r="X31" s="5">
+      <c r="X31" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -4131,7 +4132,7 @@
         <v>3</v>
       </c>
       <c r="AD31" s="3"/>
-      <c r="AE31" s="5">
+      <c r="AE31" s="4">
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
@@ -4145,15 +4146,15 @@
       <c r="AI31" s="3">
         <v>5</v>
       </c>
-      <c r="AJ31" s="5">
+      <c r="AJ31" s="4">
         <f t="shared" si="3"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="AK31" s="5">
+      <c r="AK31" s="4">
         <f t="shared" si="4"/>
         <v>4.7272727272727275</v>
       </c>
-      <c r="AL31" s="6"/>
+      <c r="AL31" s="5"/>
     </row>
     <row r="32" spans="1:38">
       <c r="A32" s="3">
@@ -4162,7 +4163,7 @@
       <c r="B32" s="3">
         <v>2</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="3">
@@ -4188,7 +4189,7 @@
       <c r="L32" s="3">
         <v>7</v>
       </c>
-      <c r="M32" s="5">
+      <c r="M32" s="4">
         <f t="shared" si="0"/>
         <v>5.5714285714285712</v>
       </c>
@@ -4220,7 +4221,7 @@
       <c r="W32" s="3">
         <v>6</v>
       </c>
-      <c r="X32" s="5">
+      <c r="X32" s="4">
         <f t="shared" si="1"/>
         <v>4.1111111111111107</v>
       </c>
@@ -4240,7 +4241,7 @@
         <v>3</v>
       </c>
       <c r="AD32" s="3"/>
-      <c r="AE32" s="5">
+      <c r="AE32" s="4">
         <f t="shared" si="2"/>
         <v>5.4</v>
       </c>
@@ -4254,15 +4255,15 @@
       <c r="AI32" s="3">
         <v>5</v>
       </c>
-      <c r="AJ32" s="5">
+      <c r="AJ32" s="4">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="AK32" s="5">
+      <c r="AK32" s="4">
         <f t="shared" si="4"/>
         <v>4.791666666666667</v>
       </c>
-      <c r="AL32" s="6"/>
+      <c r="AL32" s="5"/>
     </row>
     <row r="33" spans="1:38">
       <c r="A33" s="3">
@@ -4271,7 +4272,7 @@
       <c r="B33" s="3">
         <v>3</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="3">
@@ -4297,7 +4298,7 @@
       <c r="L33" s="3">
         <v>7</v>
       </c>
-      <c r="M33" s="5">
+      <c r="M33" s="4">
         <f t="shared" si="0"/>
         <v>5.7142857142857144</v>
       </c>
@@ -4329,7 +4330,7 @@
       <c r="W33" s="3">
         <v>6</v>
       </c>
-      <c r="X33" s="5">
+      <c r="X33" s="4">
         <f t="shared" si="1"/>
         <v>4.333333333333333</v>
       </c>
@@ -4351,7 +4352,7 @@
       <c r="AD33" s="3">
         <v>7</v>
       </c>
-      <c r="AE33" s="5">
+      <c r="AE33" s="4">
         <f t="shared" si="2"/>
         <v>5.666666666666667</v>
       </c>
@@ -4367,15 +4368,15 @@
       <c r="AI33" s="3">
         <v>6</v>
       </c>
-      <c r="AJ33" s="5">
+      <c r="AJ33" s="4">
         <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
-      <c r="AK33" s="5">
+      <c r="AK33" s="4">
         <f t="shared" si="4"/>
         <v>5.0769230769230766</v>
       </c>
-      <c r="AL33" s="6"/>
+      <c r="AL33" s="5"/>
     </row>
     <row r="34" spans="1:38">
       <c r="A34" s="3">
@@ -4384,7 +4385,7 @@
       <c r="B34" s="3">
         <v>4</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D34" s="3">
@@ -4410,7 +4411,7 @@
       <c r="L34" s="3">
         <v>7</v>
       </c>
-      <c r="M34" s="5">
+      <c r="M34" s="4">
         <f t="shared" si="0"/>
         <v>5.7142857142857144</v>
       </c>
@@ -4444,7 +4445,7 @@
       <c r="W34" s="3">
         <v>7</v>
       </c>
-      <c r="X34" s="5">
+      <c r="X34" s="4">
         <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>3</v>
       </c>
       <c r="AD34" s="3"/>
-      <c r="AE34" s="5">
+      <c r="AE34" s="4">
         <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
@@ -4478,15 +4479,15 @@
       <c r="AI34" s="3">
         <v>6</v>
       </c>
-      <c r="AJ34" s="5">
+      <c r="AJ34" s="4">
         <f t="shared" si="3"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="AK34" s="5">
+      <c r="AK34" s="4">
         <f t="shared" si="4"/>
         <v>5.12</v>
       </c>
-      <c r="AL34" s="6">
+      <c r="AL34" s="5">
         <f>AK34-AK31</f>
         <v>0.39272727272727259</v>
       </c>
@@ -4498,7 +4499,7 @@
       <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D35" s="3">
@@ -4524,7 +4525,7 @@
       <c r="L35" s="3">
         <v>5</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M35" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -4554,7 +4555,7 @@
         <v>4</v>
       </c>
       <c r="W35" s="3"/>
-      <c r="X35" s="5">
+      <c r="X35" s="4">
         <f t="shared" si="1"/>
         <v>4.125</v>
       </c>
@@ -4568,7 +4569,7 @@
       <c r="AB35" s="3"/>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
-      <c r="AE35" s="5">
+      <c r="AE35" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -4584,15 +4585,15 @@
       <c r="AI35" s="3">
         <v>3</v>
       </c>
-      <c r="AJ35" s="5">
+      <c r="AJ35" s="4">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AK35" s="5">
+      <c r="AK35" s="4">
         <f t="shared" si="4"/>
         <v>4.6190476190476186</v>
       </c>
-      <c r="AL35" s="6"/>
+      <c r="AL35" s="5"/>
     </row>
     <row r="36" spans="1:38">
       <c r="A36" s="3">
@@ -4601,7 +4602,7 @@
       <c r="B36" s="3">
         <v>2</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D36" s="3">
@@ -4627,7 +4628,7 @@
       <c r="L36" s="3">
         <v>5</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="4">
         <f t="shared" si="0"/>
         <v>6.2857142857142856</v>
       </c>
@@ -4657,7 +4658,7 @@
         <v>4</v>
       </c>
       <c r="W36" s="3"/>
-      <c r="X36" s="5">
+      <c r="X36" s="4">
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
@@ -4673,7 +4674,7 @@
         <v>6</v>
       </c>
       <c r="AD36" s="3"/>
-      <c r="AE36" s="5">
+      <c r="AE36" s="4">
         <f t="shared" si="2"/>
         <v>3.6666666666666665</v>
       </c>
@@ -4689,15 +4690,15 @@
       <c r="AI36" s="3">
         <v>4</v>
       </c>
-      <c r="AJ36" s="5">
+      <c r="AJ36" s="4">
         <f t="shared" si="3"/>
         <v>5.25</v>
       </c>
-      <c r="AK36" s="5">
+      <c r="AK36" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="AL36" s="6"/>
+      <c r="AL36" s="5"/>
     </row>
     <row r="37" spans="1:38">
       <c r="A37" s="3">
@@ -4706,7 +4707,7 @@
       <c r="B37" s="3">
         <v>4</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D37" s="3">
@@ -4732,7 +4733,7 @@
       <c r="L37" s="3">
         <v>5</v>
       </c>
-      <c r="M37" s="5">
+      <c r="M37" s="4">
         <f t="shared" si="0"/>
         <v>6.4285714285714288</v>
       </c>
@@ -4764,7 +4765,7 @@
       <c r="W37" s="3">
         <v>7</v>
       </c>
-      <c r="X37" s="5">
+      <c r="X37" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -4782,7 +4783,7 @@
         <v>6</v>
       </c>
       <c r="AD37" s="3"/>
-      <c r="AE37" s="5">
+      <c r="AE37" s="4">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
@@ -4798,15 +4799,15 @@
       <c r="AI37" s="3">
         <v>4</v>
       </c>
-      <c r="AJ37" s="5">
+      <c r="AJ37" s="4">
         <f t="shared" si="3"/>
         <v>5.5</v>
       </c>
-      <c r="AK37" s="5">
+      <c r="AK37" s="4">
         <f t="shared" si="4"/>
         <v>5.25</v>
       </c>
-      <c r="AL37" s="6">
+      <c r="AL37" s="5">
         <f>AK37-AK35</f>
         <v>0.63095238095238138</v>
       </c>
@@ -4818,7 +4819,7 @@
       <c r="B38" s="3">
         <v>1</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D38" s="3">
@@ -4846,7 +4847,7 @@
       <c r="L38" s="3">
         <v>6</v>
       </c>
-      <c r="M38" s="5">
+      <c r="M38" s="4">
         <f t="shared" si="0"/>
         <v>6.125</v>
       </c>
@@ -4878,7 +4879,7 @@
       <c r="W38" s="3">
         <v>5</v>
       </c>
-      <c r="X38" s="5">
+      <c r="X38" s="4">
         <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
@@ -4896,7 +4897,7 @@
       <c r="AD38" s="3">
         <v>8</v>
       </c>
-      <c r="AE38" s="5">
+      <c r="AE38" s="4">
         <f t="shared" si="2"/>
         <v>4.75</v>
       </c>
@@ -4912,15 +4913,15 @@
       <c r="AI38" s="3">
         <v>4</v>
       </c>
-      <c r="AJ38" s="5">
+      <c r="AJ38" s="4">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="AK38" s="5">
+      <c r="AK38" s="4">
         <f t="shared" si="4"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="AL38" s="6"/>
+      <c r="AL38" s="5"/>
     </row>
     <row r="39" spans="1:38">
       <c r="A39" s="3">
@@ -4929,7 +4930,7 @@
       <c r="B39" s="3">
         <v>2</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="3">
@@ -4955,7 +4956,7 @@
       <c r="L39" s="3">
         <v>6</v>
       </c>
-      <c r="M39" s="5">
+      <c r="M39" s="4">
         <f t="shared" si="0"/>
         <v>6.4285714285714288</v>
       </c>
@@ -4987,7 +4988,7 @@
       <c r="W39" s="3">
         <v>5</v>
       </c>
-      <c r="X39" s="5">
+      <c r="X39" s="4">
         <f t="shared" si="1"/>
         <v>3.5555555555555554</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>5</v>
       </c>
       <c r="AD39" s="3"/>
-      <c r="AE39" s="5">
+      <c r="AE39" s="4">
         <f t="shared" si="2"/>
         <v>4.25</v>
       </c>
@@ -5021,15 +5022,15 @@
       <c r="AI39" s="3">
         <v>6</v>
       </c>
-      <c r="AJ39" s="5">
+      <c r="AJ39" s="4">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="AK39" s="5">
+      <c r="AK39" s="4">
         <f t="shared" si="4"/>
         <v>4.583333333333333</v>
       </c>
-      <c r="AL39" s="6"/>
+      <c r="AL39" s="5"/>
     </row>
     <row r="40" spans="1:38">
       <c r="A40" s="3">
@@ -5038,7 +5039,7 @@
       <c r="B40" s="3">
         <v>3</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="3">
@@ -5064,7 +5065,7 @@
       <c r="L40" s="3">
         <v>6</v>
       </c>
-      <c r="M40" s="5">
+      <c r="M40" s="4">
         <f t="shared" si="0"/>
         <v>6.4285714285714288</v>
       </c>
@@ -5092,7 +5093,7 @@
       <c r="W40" s="3">
         <v>5</v>
       </c>
-      <c r="X40" s="5">
+      <c r="X40" s="4">
         <f t="shared" si="1"/>
         <v>5.1428571428571432</v>
       </c>
@@ -5110,7 +5111,7 @@
         <v>5</v>
       </c>
       <c r="AD40" s="3"/>
-      <c r="AE40" s="5">
+      <c r="AE40" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -5126,15 +5127,15 @@
       <c r="AI40" s="3">
         <v>6</v>
       </c>
-      <c r="AJ40" s="5">
+      <c r="AJ40" s="4">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="AK40" s="5">
+      <c r="AK40" s="4">
         <f t="shared" si="4"/>
         <v>5.3181818181818183</v>
       </c>
-      <c r="AL40" s="6"/>
+      <c r="AL40" s="5"/>
     </row>
     <row r="41" spans="1:38">
       <c r="A41" s="3">
@@ -5143,7 +5144,7 @@
       <c r="B41" s="3">
         <v>4</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D41" s="3">
@@ -5169,7 +5170,7 @@
       <c r="L41" s="3">
         <v>6</v>
       </c>
-      <c r="M41" s="5">
+      <c r="M41" s="4">
         <f t="shared" si="0"/>
         <v>6.5714285714285712</v>
       </c>
@@ -5203,7 +5204,7 @@
       <c r="W41" s="3">
         <v>4</v>
       </c>
-      <c r="X41" s="5">
+      <c r="X41" s="4">
         <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>5</v>
       </c>
       <c r="AD41" s="3"/>
-      <c r="AE41" s="5">
+      <c r="AE41" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -5231,15 +5232,15 @@
       <c r="AI41" s="3">
         <v>6</v>
       </c>
-      <c r="AJ41" s="5">
+      <c r="AJ41" s="4">
         <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
-      <c r="AK41" s="5">
+      <c r="AK41" s="4">
         <f t="shared" si="4"/>
         <v>5.7272727272727275</v>
       </c>
-      <c r="AL41" s="6"/>
+      <c r="AL41" s="5"/>
     </row>
     <row r="42" spans="1:38">
       <c r="A42" s="3">
@@ -5248,7 +5249,7 @@
       <c r="B42" s="3">
         <v>5</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D42" s="3"/>
@@ -5266,7 +5267,7 @@
       <c r="L42" s="3">
         <v>7</v>
       </c>
-      <c r="M42" s="5">
+      <c r="M42" s="4">
         <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
@@ -5294,7 +5295,7 @@
       <c r="W42" s="3">
         <v>3</v>
       </c>
-      <c r="X42" s="5">
+      <c r="X42" s="4">
         <f t="shared" si="1"/>
         <v>4.8571428571428568</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>4</v>
       </c>
       <c r="AD42" s="3"/>
-      <c r="AE42" s="5">
+      <c r="AE42" s="4">
         <f t="shared" si="2"/>
         <v>4.666666666666667</v>
       </c>
@@ -5326,15 +5327,15 @@
       <c r="AI42" s="3">
         <v>6</v>
       </c>
-      <c r="AJ42" s="5">
+      <c r="AJ42" s="4">
         <f t="shared" si="3"/>
         <v>4.75</v>
       </c>
-      <c r="AK42" s="5">
+      <c r="AK42" s="4">
         <f t="shared" si="4"/>
         <v>5.117647058823529</v>
       </c>
-      <c r="AL42" s="6">
+      <c r="AL42" s="5">
         <f>AK42-AK38</f>
         <v>0.71764705882352864</v>
       </c>
@@ -5346,7 +5347,7 @@
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D43" s="3">
@@ -5372,7 +5373,7 @@
       <c r="L43" s="3">
         <v>2</v>
       </c>
-      <c r="M43" s="5">
+      <c r="M43" s="4">
         <f t="shared" si="0"/>
         <v>3.4285714285714284</v>
       </c>
@@ -5406,7 +5407,7 @@
       <c r="W43" s="3">
         <v>6</v>
       </c>
-      <c r="X43" s="5">
+      <c r="X43" s="4">
         <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
@@ -5426,7 +5427,7 @@
         <v>0</v>
       </c>
       <c r="AD43" s="3"/>
-      <c r="AE43" s="5">
+      <c r="AE43" s="4">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
@@ -5442,15 +5443,15 @@
       <c r="AI43" s="3">
         <v>5</v>
       </c>
-      <c r="AJ43" s="5">
+      <c r="AJ43" s="4">
         <f t="shared" si="3"/>
         <v>5.75</v>
       </c>
-      <c r="AK43" s="5">
+      <c r="AK43" s="4">
         <f t="shared" si="4"/>
         <v>3.8461538461538463</v>
       </c>
-      <c r="AL43" s="6"/>
+      <c r="AL43" s="5"/>
     </row>
     <row r="44" spans="1:38">
       <c r="A44" s="3">
@@ -5459,7 +5460,7 @@
       <c r="B44" s="3">
         <v>2</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D44" s="3">
@@ -5485,7 +5486,7 @@
       <c r="L44" s="3">
         <v>2</v>
       </c>
-      <c r="M44" s="5">
+      <c r="M44" s="4">
         <f t="shared" si="0"/>
         <v>3.4285714285714284</v>
       </c>
@@ -5519,7 +5520,7 @@
       <c r="W44" s="3">
         <v>8</v>
       </c>
-      <c r="X44" s="5">
+      <c r="X44" s="4">
         <f t="shared" si="1"/>
         <v>3.2</v>
       </c>
@@ -5535,7 +5536,7 @@
       </c>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
-      <c r="AE44" s="5">
+      <c r="AE44" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -5549,15 +5550,15 @@
       <c r="AI44" s="3">
         <v>8</v>
       </c>
-      <c r="AJ44" s="5">
+      <c r="AJ44" s="4">
         <f t="shared" si="3"/>
         <v>5.666666666666667</v>
       </c>
-      <c r="AK44" s="5">
+      <c r="AK44" s="4">
         <f t="shared" si="4"/>
         <v>3.4347826086956523</v>
       </c>
-      <c r="AL44" s="6"/>
+      <c r="AL44" s="5"/>
     </row>
     <row r="45" spans="1:38">
       <c r="A45" s="3">
@@ -5566,7 +5567,7 @@
       <c r="B45" s="3">
         <v>4</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D45" s="3">
@@ -5592,7 +5593,7 @@
       <c r="L45" s="3">
         <v>1</v>
       </c>
-      <c r="M45" s="5">
+      <c r="M45" s="4">
         <f t="shared" si="0"/>
         <v>2.8571428571428572</v>
       </c>
@@ -5626,7 +5627,7 @@
       <c r="W45" s="3">
         <v>3</v>
       </c>
-      <c r="X45" s="5">
+      <c r="X45" s="4">
         <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
@@ -5644,7 +5645,7 @@
       <c r="AD45" s="3">
         <v>7</v>
       </c>
-      <c r="AE45" s="5">
+      <c r="AE45" s="4">
         <f t="shared" si="2"/>
         <v>3.25</v>
       </c>
@@ -5660,15 +5661,15 @@
       <c r="AI45" s="3">
         <v>5</v>
       </c>
-      <c r="AJ45" s="5">
+      <c r="AJ45" s="4">
         <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
-      <c r="AK45" s="5">
+      <c r="AK45" s="4">
         <f t="shared" si="4"/>
         <v>2.96</v>
       </c>
-      <c r="AL45" s="6"/>
+      <c r="AL45" s="5"/>
     </row>
     <row r="46" spans="1:38">
       <c r="A46" s="3">
@@ -5677,7 +5678,7 @@
       <c r="B46" s="3">
         <v>5</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D46" s="3"/>
@@ -5701,7 +5702,7 @@
       <c r="L46" s="3">
         <v>4</v>
       </c>
-      <c r="M46" s="5">
+      <c r="M46" s="4">
         <f t="shared" si="0"/>
         <v>4.833333333333333</v>
       </c>
@@ -5731,7 +5732,7 @@
         <v>3</v>
       </c>
       <c r="W46" s="3"/>
-      <c r="X46" s="5">
+      <c r="X46" s="4">
         <f t="shared" si="1"/>
         <v>3.25</v>
       </c>
@@ -5745,7 +5746,7 @@
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
-      <c r="AE46" s="5">
+      <c r="AE46" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -5761,15 +5762,15 @@
       <c r="AI46" s="3">
         <v>7</v>
       </c>
-      <c r="AJ46" s="5">
+      <c r="AJ46" s="4">
         <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
-      <c r="AK46" s="5">
+      <c r="AK46" s="4">
         <f t="shared" si="4"/>
         <v>4.25</v>
       </c>
-      <c r="AL46" s="6">
+      <c r="AL46" s="5">
         <f>AK46-AK43</f>
         <v>0.40384615384615374</v>
       </c>
@@ -5781,7 +5782,7 @@
       <c r="B47" s="3">
         <v>1</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D47" s="3">
@@ -5809,7 +5810,7 @@
       <c r="L47" s="3">
         <v>9</v>
       </c>
-      <c r="M47" s="5">
+      <c r="M47" s="4">
         <f t="shared" si="0"/>
         <v>8.375</v>
       </c>
@@ -5843,7 +5844,7 @@
       <c r="W47" s="3">
         <v>8</v>
       </c>
-      <c r="X47" s="5">
+      <c r="X47" s="4">
         <f t="shared" si="1"/>
         <v>5.7</v>
       </c>
@@ -5861,7 +5862,7 @@
       <c r="AD47" s="3">
         <v>8</v>
       </c>
-      <c r="AE47" s="5">
+      <c r="AE47" s="4">
         <f t="shared" si="2"/>
         <v>5.75</v>
       </c>
@@ -5877,15 +5878,15 @@
       <c r="AI47" s="3">
         <v>8</v>
       </c>
-      <c r="AJ47" s="5">
+      <c r="AJ47" s="4">
         <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
-      <c r="AK47" s="5">
+      <c r="AK47" s="4">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="AL47" s="6"/>
+      <c r="AL47" s="5"/>
     </row>
     <row r="48" spans="1:38">
       <c r="A48" s="3">
@@ -5894,7 +5895,7 @@
       <c r="B48" s="3">
         <v>2</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D48" s="3">
@@ -5920,7 +5921,7 @@
       <c r="L48" s="3">
         <v>8</v>
       </c>
-      <c r="M48" s="5">
+      <c r="M48" s="4">
         <f t="shared" si="0"/>
         <v>8.2857142857142865</v>
       </c>
@@ -5954,7 +5955,7 @@
       <c r="W48" s="3">
         <v>8</v>
       </c>
-      <c r="X48" s="5">
+      <c r="X48" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -5974,7 +5975,7 @@
       <c r="AD48" s="3">
         <v>8</v>
       </c>
-      <c r="AE48" s="5">
+      <c r="AE48" s="4">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -5990,15 +5991,15 @@
       <c r="AI48" s="3">
         <v>8</v>
       </c>
-      <c r="AJ48" s="5">
+      <c r="AJ48" s="4">
         <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
-      <c r="AK48" s="5">
+      <c r="AK48" s="4">
         <f t="shared" si="4"/>
         <v>7.384615384615385</v>
       </c>
-      <c r="AL48" s="6"/>
+      <c r="AL48" s="5"/>
     </row>
     <row r="49" spans="1:38">
       <c r="A49" s="3">
@@ -6007,7 +6008,7 @@
       <c r="B49" s="3">
         <v>3</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="3">
@@ -6033,7 +6034,7 @@
       <c r="L49" s="3">
         <v>9</v>
       </c>
-      <c r="M49" s="5">
+      <c r="M49" s="4">
         <f t="shared" si="0"/>
         <v>8.8571428571428577</v>
       </c>
@@ -6067,7 +6068,7 @@
       <c r="W49" s="3">
         <v>8</v>
       </c>
-      <c r="X49" s="5">
+      <c r="X49" s="4">
         <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
@@ -6085,7 +6086,7 @@
       <c r="AD49" s="3">
         <v>8</v>
       </c>
-      <c r="AE49" s="5">
+      <c r="AE49" s="4">
         <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
@@ -6101,15 +6102,15 @@
       <c r="AI49" s="3">
         <v>7</v>
       </c>
-      <c r="AJ49" s="5">
+      <c r="AJ49" s="4">
         <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
-      <c r="AK49" s="5">
+      <c r="AK49" s="4">
         <f t="shared" si="4"/>
         <v>7.84</v>
       </c>
-      <c r="AL49" s="6"/>
+      <c r="AL49" s="5"/>
     </row>
     <row r="50" spans="1:38">
       <c r="A50" s="3">
@@ -6118,7 +6119,7 @@
       <c r="B50" s="3">
         <v>4</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D50" s="3">
@@ -6144,7 +6145,7 @@
       <c r="L50" s="3">
         <v>8</v>
       </c>
-      <c r="M50" s="5">
+      <c r="M50" s="4">
         <f t="shared" si="0"/>
         <v>8.5714285714285712</v>
       </c>
@@ -6178,7 +6179,7 @@
       <c r="W50" s="3">
         <v>8</v>
       </c>
-      <c r="X50" s="5">
+      <c r="X50" s="4">
         <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
@@ -6194,7 +6195,7 @@
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
-      <c r="AE50" s="5">
+      <c r="AE50" s="4">
         <f t="shared" si="2"/>
         <v>6.333333333333333</v>
       </c>
@@ -6210,15 +6211,15 @@
       <c r="AI50" s="3">
         <v>8</v>
       </c>
-      <c r="AJ50" s="5">
+      <c r="AJ50" s="4">
         <f t="shared" si="3"/>
         <v>8.75</v>
       </c>
-      <c r="AK50" s="5">
+      <c r="AK50" s="4">
         <f t="shared" si="4"/>
         <v>7.083333333333333</v>
       </c>
-      <c r="AL50" s="6"/>
+      <c r="AL50" s="5"/>
     </row>
     <row r="51" spans="1:38">
       <c r="A51" s="3">
@@ -6227,7 +6228,7 @@
       <c r="B51" s="3">
         <v>5</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="3"/>
@@ -6251,7 +6252,7 @@
       <c r="L51" s="3">
         <v>9</v>
       </c>
-      <c r="M51" s="5">
+      <c r="M51" s="4">
         <f t="shared" si="0"/>
         <v>8.8333333333333339</v>
       </c>
@@ -6285,7 +6286,7 @@
       <c r="W51" s="3">
         <v>9</v>
       </c>
-      <c r="X51" s="5">
+      <c r="X51" s="4">
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
@@ -6301,7 +6302,7 @@
       <c r="AD51" s="3">
         <v>7</v>
       </c>
-      <c r="AE51" s="5">
+      <c r="AE51" s="4">
         <f t="shared" si="2"/>
         <v>7.333333333333333</v>
       </c>
@@ -6317,15 +6318,15 @@
       <c r="AI51" s="3">
         <v>9</v>
       </c>
-      <c r="AJ51" s="5">
+      <c r="AJ51" s="4">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="AK51" s="5">
+      <c r="AK51" s="4">
         <f t="shared" si="4"/>
         <v>7.5217391304347823</v>
       </c>
-      <c r="AL51" s="6">
+      <c r="AL51" s="5">
         <f>AK51-AK47</f>
         <v>0.52173913043478226</v>
       </c>

</xml_diff>

<commit_message>
Change Control Group Name
</commit_message>
<xml_diff>
--- a/Base_Data/Excel+ALL+ENG.xlsx
+++ b/Base_Data/Excel+ALL+ENG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex.y/Documents/Github_Repo/G10_CTB_Global-Finals_Data-Analysis/Base_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex.y/Documents/Github_Repo/CTB24-25_Global-Finals_Data-Analysis_Graphing/Base_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6469CB88-29BA-1E48-A0EB-1BB918114B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC425CB-E2BA-7D46-BACB-40069AECDD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="31720" windowHeight="22500" xr2:uid="{98D09DEC-93DB-E744-8CBC-B24D25E4341D}"/>
   </bookViews>
@@ -170,10 +170,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Non-Accompanied Group</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Learning Behaviors and Classroom Adaptation Mean Score</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,6 +191,10 @@
   </si>
   <si>
     <t>Overall Daily Performance Mean Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control Group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0A3F08-FF35-D14B-A48B-730CB434908B}">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -751,7 +751,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
@@ -784,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>19</v>
@@ -805,7 +805,7 @@
         <v>24</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>25</v>
@@ -820,13 +820,13 @@
         <v>28</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AK1" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AL1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -4056,7 +4056,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D31" s="3">
         <v>9</v>
@@ -4161,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D32" s="3">
         <v>9</v>
@@ -4270,7 +4270,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D33" s="3">
         <v>9</v>
@@ -4383,7 +4383,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D34" s="3">
         <v>9</v>
@@ -4497,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D35" s="3">
         <v>8</v>
@@ -4600,7 +4600,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D36" s="3">
         <v>8</v>
@@ -4705,7 +4705,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D37" s="3">
         <v>8</v>
@@ -4817,7 +4817,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D38" s="3">
         <v>8</v>
@@ -4928,7 +4928,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D39" s="3">
         <v>8</v>
@@ -5037,7 +5037,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D40" s="3">
         <v>8</v>
@@ -5142,7 +5142,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D41" s="3">
         <v>8</v>
@@ -5247,7 +5247,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -5345,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -5458,7 +5458,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D44" s="3">
         <v>3</v>
@@ -5565,7 +5565,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D45" s="3">
         <v>5</v>
@@ -5676,7 +5676,7 @@
         <v>5</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3">
@@ -5780,7 +5780,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D47" s="3">
         <v>8</v>
@@ -5893,7 +5893,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D48" s="3">
         <v>8</v>
@@ -6006,7 +6006,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D49" s="3">
         <v>8</v>
@@ -6117,7 +6117,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D50" s="3">
         <v>9</v>
@@ -6226,7 +6226,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3">

</xml_diff>

<commit_message>
Shorten "Difference in Mean Performance Scores....."
</commit_message>
<xml_diff>
--- a/Base_Data/Excel+ALL+ENG.xlsx
+++ b/Base_Data/Excel+ALL+ENG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex.y/Documents/Github_Repo/CTB24-25_Global-Finals_Data-Analysis_Graphing/Base_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC425CB-E2BA-7D46-BACB-40069AECDD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE0C808-EB82-1F40-9FE2-9E1693035EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="31720" windowHeight="22500" xr2:uid="{98D09DEC-93DB-E744-8CBC-B24D25E4341D}"/>
   </bookViews>
@@ -170,31 +170,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Learning Behaviors and Classroom Adaptation Mean Score</t>
+    <t>Control Group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Emotion Regulation Mean Score</t>
+    <t>Learning Behaviors and Classroom Adaptation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Difference in Mean Performance Scores Pre- and Post-Intervention</t>
+    <t>Social Interaction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Repetitive Behaviors and Interests Mean Score</t>
+    <t>Emotion Regulation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Social Interaction Mean Score</t>
+    <t>Repetitive Behaviors and Interests</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Overall Daily Performance Mean Score</t>
+    <t>Overall Daily Performance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Control Group</t>
+    <t>Difference in Mean Performance Scores</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0A3F08-FF35-D14B-A48B-730CB434908B}">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="AJ10" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -751,7 +751,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
@@ -784,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>19</v>
@@ -805,7 +805,7 @@
         <v>24</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>25</v>
@@ -820,13 +820,13 @@
         <v>28</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AK1" s="7" t="s">
         <v>38</v>
       </c>
       <c r="AL1" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -4056,7 +4056,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D31" s="3">
         <v>9</v>
@@ -4161,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D32" s="3">
         <v>9</v>
@@ -4270,7 +4270,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3">
         <v>9</v>
@@ -4383,7 +4383,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D34" s="3">
         <v>9</v>
@@ -4497,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D35" s="3">
         <v>8</v>
@@ -4600,7 +4600,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D36" s="3">
         <v>8</v>
@@ -4705,7 +4705,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D37" s="3">
         <v>8</v>
@@ -4817,7 +4817,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D38" s="3">
         <v>8</v>
@@ -4928,7 +4928,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D39" s="3">
         <v>8</v>
@@ -5037,7 +5037,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D40" s="3">
         <v>8</v>
@@ -5142,7 +5142,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D41" s="3">
         <v>8</v>
@@ -5247,7 +5247,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -5345,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -5458,7 +5458,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D44" s="3">
         <v>3</v>
@@ -5565,7 +5565,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D45" s="3">
         <v>5</v>
@@ -5676,7 +5676,7 @@
         <v>5</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3">
@@ -5780,7 +5780,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D47" s="3">
         <v>8</v>
@@ -5893,7 +5893,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D48" s="3">
         <v>8</v>
@@ -6006,7 +6006,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D49" s="3">
         <v>8</v>
@@ -6117,7 +6117,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D50" s="3">
         <v>9</v>
@@ -6226,7 +6226,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3">

</xml_diff>